<commit_message>
Working solution of the API
</commit_message>
<xml_diff>
--- a/ExcelUtility/Queries.xlsx
+++ b/ExcelUtility/Queries.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Reqid</t>
   </si>
@@ -70,7 +70,67 @@
     <t>How are you ?</t>
   </si>
   <si>
+    <t>Something something</t>
+  </si>
+  <si>
+    <t>22962f26-a8ad-4c36-b5eb-9449d90c0ed4</t>
+  </si>
+  <si>
+    <t>Mahesh</t>
+  </si>
+  <si>
+    <t>977448714</t>
+  </si>
+  <si>
+    <t>maheshanna@gmail.com</t>
+  </si>
+  <si>
+    <t>I am good!!</t>
+  </si>
+  <si>
+    <t>12962f26-a8ad-4c36-b5eb-9449d90c0ed4</t>
+  </si>
+  <si>
+    <t>Jamanalal</t>
+  </si>
+  <si>
+    <t>977448724</t>
+  </si>
+  <si>
+    <t>What are the data</t>
+  </si>
+  <si>
+    <t>54ebd306-48fd-49f9-b7c5-ffb134f0dd77</t>
+  </si>
+  <si>
+    <t>fadsf</t>
+  </si>
+  <si>
+    <t>adsfa</t>
+  </si>
+  <si>
+    <t>fasdfa</t>
+  </si>
+  <si>
+    <t>afasfaf</t>
+  </si>
+  <si>
     <t/>
+  </si>
+  <si>
+    <t>4b4ce39b-75bd-4afd-839d-2ac907064aa8</t>
+  </si>
+  <si>
+    <t>Biraj Dey</t>
+  </si>
+  <si>
+    <t>8789445445</t>
+  </si>
+  <si>
+    <t>biraj123@gmail.com</t>
+  </si>
+  <si>
+    <t>sdfkajflksd</t>
   </si>
 </sst>
 </file>
@@ -413,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -495,6 +555,98 @@
         <v>18</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>